<commit_message>
Changes to constrains + color change in vac when warning
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F60B59C-FCAE-4932-A29F-CBCFC832B8D3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D59A7-2C8C-4496-A01F-22FD85BD0999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="227">
   <si>
     <t>clause</t>
   </si>
@@ -278,9 +278,6 @@
     <t>&lt;p&gt;You are at the end of the questionaire: &lt;/p&gt;&lt;p&gt;"{{display_field}}"&lt;/p&gt;&lt;hr&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Você finalizou o questionário por esta criança: &lt;/p&gt;&lt;p&gt;"{{display_field}}"&lt;/p&gt;&lt;hr&gt;</t>
-  </si>
-  <si>
     <t>finalize_survey_button_label</t>
   </si>
   <si>
@@ -620,12 +617,6 @@
     <t>'?' + odkSurvey.getHashString('MIF')</t>
   </si>
   <si>
-    <t>Woman in the fertile age - visit</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - visita</t>
-  </si>
-  <si>
     <t>Choose a form</t>
   </si>
   <si>
@@ -659,75 +650,30 @@
     <t>'?' + odkSurvey.getHashString('TEST')</t>
   </si>
   <si>
-    <t>Child Visit</t>
-  </si>
-  <si>
-    <t>SCAR</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('SCAR')</t>
-  </si>
-  <si>
     <t>CRIANCA</t>
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('CRIANCA')</t>
   </si>
   <si>
-    <t>GRAVIDA</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('GRAVIDA')</t>
-  </si>
-  <si>
     <t>GRAVIDA_VISIT</t>
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('GRAVIDA_VISIT')</t>
   </si>
   <si>
-    <t>CRIANCA_VISIT</t>
-  </si>
-  <si>
     <t>SES</t>
   </si>
   <si>
     <t>'?' + odkSurvey.getHashString('SES')</t>
   </si>
   <si>
-    <t>'?' + odkSurvey.getHashString('CRIANCA_VISIT')</t>
-  </si>
-  <si>
-    <t>VAC</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('VAC')</t>
-  </si>
-  <si>
     <t xml:space="preserve">Woman in the fertile age </t>
   </si>
   <si>
-    <t>Vaccine</t>
-  </si>
-  <si>
-    <t>Scars</t>
-  </si>
-  <si>
-    <t>Cicatrizes</t>
-  </si>
-  <si>
-    <t>Mulher na idade fertil - visitas</t>
-  </si>
-  <si>
     <t>Mulher na idade fertil</t>
   </si>
   <si>
-    <t>Pregnant</t>
-  </si>
-  <si>
-    <t>Grávidas</t>
-  </si>
-  <si>
     <t>Pregnants_visits</t>
   </si>
   <si>
@@ -740,13 +686,25 @@
     <t>Child</t>
   </si>
   <si>
-    <t>Crianca_visitas</t>
-  </si>
-  <si>
-    <t>MIF_VISIT</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('MIF_VISIT')</t>
+    <t>CRIANCA_HOSP</t>
+  </si>
+  <si>
+    <t>Child hospitalization</t>
+  </si>
+  <si>
+    <t>MORSLIST</t>
+  </si>
+  <si>
+    <t>MORLIST</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('MORLIST')</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('CRIANCA_HOSP')</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Você finalizou o questionário: &lt;/p&gt;&lt;p&gt;"{{display_field}}"&lt;/p&gt;&lt;hr&gt;</t>
   </si>
 </sst>
 </file>
@@ -804,7 +762,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -813,13 +771,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1130,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B793DC04-5EE8-4C44-A7FC-F90344029075}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1152,16 +1108,16 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1193,37 +1149,37 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F6" t="s">
         <v>174</v>
-      </c>
-      <c r="F6" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="E7" t="s">
+        <v>171</v>
+      </c>
+      <c r="F7" t="s">
         <v>172</v>
-      </c>
-      <c r="F7" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -1233,29 +1189,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>178</v>
-      </c>
       <c r="C1" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -1263,142 +1219,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B2" t="s">
         <v>195</v>
       </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
       <c r="C2" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="D2" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
       <c r="D3" t="s">
-        <v>199</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="C4" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="D4" t="s">
-        <v>230</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D6" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B7" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C7" t="s">
-        <v>232</v>
+        <v>205</v>
       </c>
       <c r="D7" t="s">
-        <v>233</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
       <c r="C8" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D8" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>195</v>
-      </c>
-      <c r="B9" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" t="s">
-        <v>208</v>
-      </c>
-      <c r="D9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>195</v>
-      </c>
-      <c r="B10" t="s">
-        <v>220</v>
-      </c>
-      <c r="C10" t="s">
-        <v>211</v>
-      </c>
-      <c r="D10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>195</v>
-      </c>
-      <c r="B11" t="s">
-        <v>214</v>
-      </c>
-      <c r="C11" t="s">
-        <v>237</v>
-      </c>
-      <c r="D11" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1408,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46EC045-695E-47E3-9856-F3F6A59BF71E}">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,277 +1341,214 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" t="s">
         <v>185</v>
-      </c>
-      <c r="D2" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
+        <v>188</v>
+      </c>
+      <c r="G5" t="s">
         <v>189</v>
-      </c>
-      <c r="G5" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="5" t="s">
-        <v>197</v>
-      </c>
       <c r="E9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G9" t="s">
         <v>193</v>
-      </c>
-      <c r="G9" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="5" t="s">
-        <v>240</v>
+      <c r="B12" s="4" t="s">
+        <v>209</v>
       </c>
       <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="G12" t="s">
         <v>193</v>
-      </c>
-      <c r="G12" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="5" t="s">
-        <v>225</v>
+      <c r="B15" s="4" t="s">
+        <v>211</v>
       </c>
       <c r="E15" t="s">
+        <v>192</v>
+      </c>
+      <c r="G15" t="s">
         <v>193</v>
-      </c>
-      <c r="G15" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>212</v>
+        <v>220</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="5" t="s">
-        <v>213</v>
+      <c r="B18" s="4" t="s">
+        <v>225</v>
       </c>
       <c r="E18" t="s">
+        <v>192</v>
+      </c>
+      <c r="G18" t="s">
         <v>193</v>
-      </c>
-      <c r="G18" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>215</v>
+      <c r="B21" s="4" t="s">
+        <v>213</v>
       </c>
       <c r="E21" t="s">
+        <v>192</v>
+      </c>
+      <c r="G21" t="s">
         <v>193</v>
-      </c>
-      <c r="G21" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="5" t="s">
-        <v>217</v>
+      <c r="B24" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="E24" t="s">
+        <v>192</v>
+      </c>
+      <c r="G24" t="s">
         <v>193</v>
-      </c>
-      <c r="G24" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="5" t="s">
-        <v>219</v>
+      <c r="B27" s="4" t="s">
+        <v>224</v>
       </c>
       <c r="E27" t="s">
+        <v>192</v>
+      </c>
+      <c r="G27" t="s">
         <v>193</v>
-      </c>
-      <c r="G27" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="E30" t="s">
-        <v>193</v>
-      </c>
-      <c r="G30" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B33" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="E33" t="s">
-        <v>193</v>
-      </c>
-      <c r="G33" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B36" s="5" t="s">
-        <v>222</v>
-      </c>
-      <c r="E36" t="s">
-        <v>193</v>
-      </c>
-      <c r="G36" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C37" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1709,655 +1560,655 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="57.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="56.140625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="56.140625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C5" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>206</v>
+      <c r="C6" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>206</v>
+      <c r="C7" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="C13" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C14" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C15" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C16" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>206</v>
+      <c r="C17" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="6" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="6" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="6" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="6" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C28" s="3"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="B30" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C30" s="2" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="B31" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="2" t="s">
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="B32" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="2" t="s">
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="B33" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C33" s="2" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="B34" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="B36" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C36" s="2" t="s">
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="B37" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="C37" s="2" t="s">
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="B38" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C38" s="2" t="s">
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="6" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="B39" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="3" t="s">
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="B40" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C40" s="2" t="s">
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="6" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="B41" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="C41" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C41" s="2" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="B42" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="2" t="s">
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="B43" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C43" s="3" t="s">
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="6" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="B44" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="6" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="B45" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="2" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="6" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="B46" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C46" s="2" t="s">
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="B47" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="C47" s="2" t="s">
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="B48" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="C48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="B49" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="3" t="s">
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="6" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="B50" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C50" s="2" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="6" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="B51" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="B51" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="B52" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="C52" s="2" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="B53" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="B53" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" s="2" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="6" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
+      <c r="B54" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="C54" s="2" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="6" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
+      <c r="B55" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="C55" s="2" t="s">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="6" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
+      <c r="B56" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="C56" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="C56" s="2" t="s">
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+      <c r="B57" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="C57" s="2" t="s">
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="B58" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="C58" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="C58" s="2" t="s">
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
+      <c r="B59" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="C59" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New pregnancy table (once again.......)
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055D59A7-2C8C-4496-A01F-22FD85BD0999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABFA819-1E26-4E13-8B81-38DC9A87B083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="228">
   <si>
     <t>clause</t>
   </si>
@@ -674,12 +674,6 @@
     <t>Mulher na idade fertil</t>
   </si>
   <si>
-    <t>Pregnants_visits</t>
-  </si>
-  <si>
-    <t>Grávidas_visitas</t>
-  </si>
-  <si>
     <t>Crianca</t>
   </si>
   <si>
@@ -705,6 +699,15 @@
   </si>
   <si>
     <t>&lt;p&gt;Você finalizou o questionário: &lt;/p&gt;&lt;p&gt;"{{display_field}}"&lt;/p&gt;&lt;hr&gt;</t>
+  </si>
+  <si>
+    <t>GRAVIDA</t>
+  </si>
+  <si>
+    <t>Pregnants</t>
+  </si>
+  <si>
+    <t>Grávidas</t>
   </si>
 </sst>
 </file>
@@ -1191,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1239,10 +1242,10 @@
         <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1250,13 +1253,13 @@
         <v>194</v>
       </c>
       <c r="B4" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1264,13 +1267,13 @@
         <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,13 +1309,13 @@
         <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D8" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1469,12 +1472,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E18" t="s">
         <v>192</v>
@@ -1532,12 +1535,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E27" t="s">
         <v>192</v>
@@ -1560,7 +1563,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A43F1AA-AE9E-40A3-94B1-695B21603B14}">
   <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
@@ -1882,7 +1885,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update to all model sheets
</commit_message>
<xml_diff>
--- a/app/config/assets/framework/forms/framework/framework.xlsx
+++ b/app/config/assets/framework/forms/framework/framework.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABFA819-1E26-4E13-8B81-38DC9A87B083}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD876A42-D90B-40DF-AEE8-FE6ED65DAFC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="227">
   <si>
     <t>clause</t>
   </si>
@@ -656,12 +656,6 @@
     <t>'?' + odkSurvey.getHashString('CRIANCA')</t>
   </si>
   <si>
-    <t>GRAVIDA_VISIT</t>
-  </si>
-  <si>
-    <t>'?' + odkSurvey.getHashString('GRAVIDA_VISIT')</t>
-  </si>
-  <si>
     <t>SES</t>
   </si>
   <si>
@@ -708,6 +702,9 @@
   </si>
   <si>
     <t>Grávidas</t>
+  </si>
+  <si>
+    <t>'?' + odkSurvey.getHashString('GRAVIDA')</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39009FF4-ADCA-4F52-86FD-7941672D7DFF}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1228,10 +1225,10 @@
         <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,10 +1239,10 @@
         <v>208</v>
       </c>
       <c r="C3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,13 +1250,13 @@
         <v>194</v>
       </c>
       <c r="B4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C4" t="s">
+        <v>224</v>
+      </c>
+      <c r="D4" t="s">
         <v>225</v>
-      </c>
-      <c r="C4" t="s">
-        <v>226</v>
-      </c>
-      <c r="D4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,13 +1264,13 @@
         <v>194</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1281,13 +1278,13 @@
         <v>194</v>
       </c>
       <c r="B6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D6" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,13 +1306,13 @@
         <v>194</v>
       </c>
       <c r="B8" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="D8" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -1327,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B46EC045-695E-47E3-9856-F3F6A59BF71E}">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,12 +1448,12 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>210</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="E15" t="s">
         <v>192</v>
@@ -1472,12 +1469,12 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="E18" t="s">
         <v>192</v>
@@ -1493,12 +1490,12 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E21" t="s">
         <v>192</v>
@@ -1535,12 +1532,12 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E27" t="s">
         <v>192</v>
@@ -1885,7 +1882,7 @@
         <v>83</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>